<commit_message>
API - Content - Video uploading - Refresh token
</commit_message>
<xml_diff>
--- a/SecurityMatrix.xlsx
+++ b/SecurityMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\GAI\vidmov-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E2DF89-E1BB-43BF-AB67-C82D0B314713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEF4E44-3451-400F-9DB1-2209519A165B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Authority" sheetId="1" r:id="rId1"/>
@@ -260,17 +260,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,7 +659,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -685,10 +685,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2">
@@ -714,8 +714,8 @@
       <c r="P1"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1084,20 +1084,20 @@
       <c r="P15"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="15" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="C16" s="18">
-        <v>0</v>
-      </c>
-      <c r="D16" s="18">
-        <v>1</v>
-      </c>
-      <c r="E16" s="18">
+        <v>7</v>
+      </c>
+      <c r="C16" s="16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="16">
         <v>1</v>
       </c>
       <c r="I16"/>
@@ -1124,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1144,13 +1144,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="16" t="s">
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="1">
@@ -1183,9 +1183,9 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="10" t="s">
         <v>19</v>
       </c>
@@ -1571,22 +1571,26 @@
       <c r="L15" s="14"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="17" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="12">
         <f>IF(Authority!C16=1,IF(D16=1,1,0)+IF(E16=1,2,0)+IF(F16=1,4,0)+IF(G16=1,8,0)+IF(H16=1,16,0)+IF(I16=1,32,0)+IF(J16=1,64,0)+IF(K16=1,128,0),0)</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C16" s="12">
         <f>L1-B16</f>
-        <v>255</v>
-      </c>
-      <c r="D16" s="13"/>
+        <v>238</v>
+      </c>
+      <c r="D16" s="13">
+        <v>1</v>
+      </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="H16" s="13">
+        <v>1</v>
+      </c>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
@@ -1608,7 +1612,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1627,13 +1631,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="16" t="s">
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="1">
@@ -1666,9 +1670,9 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="10" t="s">
         <v>19</v>
       </c>
@@ -1759,24 +1763,18 @@
       </c>
       <c r="B5" s="12">
         <f>IF(Authority!D5=1,IF(D5=1,1,0)+IF(E5=1,2,0)+IF(F5=1,4,0)+IF(G5=1,8,0)+IF(H5=1,16,0)+IF(I5=1,32,0)+IF(J5=1,64,0)+IF(K5=1,128,0),0)</f>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C5" s="12">
         <f>L1-B5</f>
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="D5" s="13">
         <v>1</v>
       </c>
-      <c r="E5" s="13">
-        <v>1</v>
-      </c>
-      <c r="F5" s="13">
-        <v>1</v>
-      </c>
-      <c r="G5" s="13">
-        <v>1</v>
-      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
@@ -1943,21 +1941,17 @@
       </c>
       <c r="B12" s="12">
         <f>IF(Authority!D12=1,IF(D12=1,1,0)+IF(E12=1,2,0)+IF(F12=1,4,0)+IF(G12=1,8,0)+IF(H12=1,16,0)+IF(I12=1,32,0)+IF(J12=1,64,0)+IF(K12=1,128,0),0)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C12" s="12">
         <f>L1-B12</f>
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="D12" s="13">
         <v>1</v>
       </c>
-      <c r="E12" s="13">
-        <v>1</v>
-      </c>
-      <c r="F12" s="13">
-        <v>1</v>
-      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
@@ -1971,21 +1965,17 @@
       </c>
       <c r="B13" s="12">
         <f>IF(Authority!D13=1,IF(D13=1,1,0)+IF(E13=1,2,0)+IF(F13=1,4,0)+IF(G13=1,8,0)+IF(H13=1,16,0)+IF(I13=1,32,0)+IF(J13=1,64,0)+IF(K13=1,128,0),0)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C13" s="12">
         <f>L1-B13</f>
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="D13" s="13">
         <v>1</v>
       </c>
-      <c r="E13" s="13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="13">
-        <v>1</v>
-      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
@@ -2054,7 +2044,7 @@
       <c r="L15" s="14"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="17" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="12">
@@ -2102,8 +2092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2122,13 +2112,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="16" t="s">
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="1">
@@ -2161,9 +2151,9 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="10" t="s">
         <v>19</v>
       </c>
@@ -2254,24 +2244,18 @@
       </c>
       <c r="B5" s="12">
         <f>IF(Authority!E5=1,IF(D5=1,1,0)+IF(E5=1,2,0)+IF(F5=1,4,0)+IF(G5=1,8,0)+IF(H5=1,16,0)+IF(I5=1,32,0)+IF(J5=1,64,0)+IF(K5=1,128,0),0)</f>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C5" s="12">
         <f>L1-B5</f>
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="D5" s="13">
         <v>1</v>
       </c>
-      <c r="E5" s="13">
-        <v>1</v>
-      </c>
-      <c r="F5" s="13">
-        <v>1</v>
-      </c>
-      <c r="G5" s="13">
-        <v>1</v>
-      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
@@ -2438,21 +2422,17 @@
       </c>
       <c r="B12" s="12">
         <f>IF(Authority!E12=1,IF(D12=1,1,0)+IF(E12=1,2,0)+IF(F12=1,4,0)+IF(G12=1,8,0)+IF(H12=1,16,0)+IF(I12=1,32,0)+IF(J12=1,64,0)+IF(K12=1,128,0),0)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C12" s="12">
         <f>L1-B12</f>
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="D12" s="13">
         <v>1</v>
       </c>
-      <c r="E12" s="13">
-        <v>1</v>
-      </c>
-      <c r="F12" s="13">
-        <v>1</v>
-      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
@@ -2466,21 +2446,17 @@
       </c>
       <c r="B13" s="12">
         <f>IF(Authority!E13=1,IF(D13=1,1,0)+IF(E13=1,2,0)+IF(F13=1,4,0)+IF(G13=1,8,0)+IF(H13=1,16,0)+IF(I13=1,32,0)+IF(J13=1,64,0)+IF(K13=1,128,0),0)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C13" s="12">
         <f>L1-B13</f>
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="D13" s="13">
         <v>1</v>
       </c>
-      <c r="E13" s="13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="13">
-        <v>1</v>
-      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
@@ -2549,7 +2525,7 @@
       <c r="L15" s="14"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="17" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="12">

</xml_diff>

<commit_message>
- CRUD brand (for now, Arena handle it) - Change schema main_sponsor & episode_sponsor
</commit_message>
<xml_diff>
--- a/SecurityMatrix.xlsx
+++ b/SecurityMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\GAI\vidmov-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE30E76-49EB-4B09-9743-9165380CAD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3230F71-64DA-4DDE-9AF7-56A2C01A6063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Authority" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="38">
   <si>
     <t>FEATURE</t>
   </si>
@@ -141,6 +141,9 @@
   <si>
     <t>_user</t>
   </si>
+  <si>
+    <t>brand</t>
+  </si>
 </sst>
 </file>
 
@@ -240,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -265,9 +268,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -283,6 +283,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,13 +669,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -698,10 +702,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1">
@@ -730,8 +734,8 @@
       <c r="Q1"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
@@ -764,16 +768,16 @@
         <f>IF(C3=1,1,0)+IF(D3=1,2,0)+IF(E3=1,4,0)+IF(F3=1,8,0)</f>
         <v>15</v>
       </c>
-      <c r="C3" s="13">
-        <v>1</v>
-      </c>
-      <c r="D3" s="13">
-        <v>1</v>
-      </c>
-      <c r="E3" s="13">
-        <v>1</v>
-      </c>
-      <c r="F3" s="13">
+      <c r="C3" s="12">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12">
+        <v>1</v>
+      </c>
+      <c r="F3" s="12">
         <v>1</v>
       </c>
       <c r="G3" s="9"/>
@@ -791,17 +795,17 @@
         <v>5</v>
       </c>
       <c r="B4" s="8">
-        <f t="shared" ref="B4:B23" si="0">IF(C4=1,1,0)+IF(D4=1,2,0)+IF(E4=1,4,0)+IF(F4=1,8,0)</f>
+        <f t="shared" ref="B4:B24" si="0">IF(C4=1,1,0)+IF(D4=1,2,0)+IF(E4=1,4,0)+IF(F4=1,8,0)</f>
         <v>3</v>
       </c>
-      <c r="C4" s="13">
-        <v>1</v>
-      </c>
-      <c r="D4" s="13">
-        <v>1</v>
-      </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="C4" s="12">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="9"/>
       <c r="J4"/>
       <c r="K4"/>
@@ -820,12 +824,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C5" s="13">
-        <v>1</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="C5" s="12">
+        <v>1</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="6"/>
       <c r="J5"/>
       <c r="K5"/>
@@ -844,16 +848,16 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C6" s="13">
-        <v>1</v>
-      </c>
-      <c r="D6" s="13">
-        <v>1</v>
-      </c>
-      <c r="E6" s="13">
-        <v>1</v>
-      </c>
-      <c r="F6" s="13">
+      <c r="C6" s="12">
+        <v>1</v>
+      </c>
+      <c r="D6" s="12">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="12">
         <v>1</v>
       </c>
       <c r="G6" s="6"/>
@@ -874,14 +878,14 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C7" s="13">
-        <v>1</v>
-      </c>
-      <c r="D7" s="13">
-        <v>1</v>
-      </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
+      <c r="C7" s="12">
+        <v>1</v>
+      </c>
+      <c r="D7" s="12">
+        <v>1</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
       <c r="G7" s="6"/>
       <c r="J7"/>
       <c r="K7"/>
@@ -900,12 +904,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C8" s="13">
-        <v>1</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="C8" s="12">
+        <v>1</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="6"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -924,16 +928,16 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C9" s="13">
-        <v>1</v>
-      </c>
-      <c r="D9" s="13">
-        <v>1</v>
-      </c>
-      <c r="E9" s="13">
-        <v>1</v>
-      </c>
-      <c r="F9" s="13">
+      <c r="C9" s="12">
+        <v>1</v>
+      </c>
+      <c r="D9" s="12">
+        <v>1</v>
+      </c>
+      <c r="E9" s="12">
+        <v>1</v>
+      </c>
+      <c r="F9" s="12">
         <v>1</v>
       </c>
       <c r="G9" s="6"/>
@@ -954,16 +958,16 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C10" s="13">
-        <v>1</v>
-      </c>
-      <c r="D10" s="13">
-        <v>1</v>
-      </c>
-      <c r="E10" s="13">
-        <v>1</v>
-      </c>
-      <c r="F10" s="13">
+      <c r="C10" s="12">
+        <v>1</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1</v>
+      </c>
+      <c r="E10" s="12">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12">
         <v>1</v>
       </c>
       <c r="G10" s="6"/>
@@ -984,16 +988,16 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C11" s="13">
-        <v>1</v>
-      </c>
-      <c r="D11" s="13">
-        <v>1</v>
-      </c>
-      <c r="E11" s="13">
-        <v>1</v>
-      </c>
-      <c r="F11" s="13">
+      <c r="C11" s="12">
+        <v>1</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1</v>
+      </c>
+      <c r="E11" s="12">
+        <v>1</v>
+      </c>
+      <c r="F11" s="12">
         <v>1</v>
       </c>
       <c r="G11" s="6"/>
@@ -1014,12 +1018,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C12" s="13">
-        <v>1</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="C12" s="12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
       <c r="G12" s="6"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1038,12 +1042,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C13" s="13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="C13" s="12">
+        <v>1</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
       <c r="G13" s="6"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1062,12 +1066,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C14" s="13">
-        <v>1</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="C14" s="12">
+        <v>1</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
       <c r="G14" s="6"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1086,16 +1090,16 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C15" s="13">
-        <v>1</v>
-      </c>
-      <c r="D15" s="13">
-        <v>1</v>
-      </c>
-      <c r="E15" s="13">
-        <v>1</v>
-      </c>
-      <c r="F15" s="13">
+      <c r="C15" s="12">
+        <v>1</v>
+      </c>
+      <c r="D15" s="12">
+        <v>1</v>
+      </c>
+      <c r="E15" s="12">
+        <v>1</v>
+      </c>
+      <c r="F15" s="12">
         <v>1</v>
       </c>
       <c r="G15" s="6"/>
@@ -1116,16 +1120,16 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C16" s="13">
-        <v>1</v>
-      </c>
-      <c r="D16" s="13">
-        <v>1</v>
-      </c>
-      <c r="E16" s="13">
-        <v>1</v>
-      </c>
-      <c r="F16" s="13">
+      <c r="C16" s="12">
+        <v>1</v>
+      </c>
+      <c r="D16" s="12">
+        <v>1</v>
+      </c>
+      <c r="E16" s="12">
+        <v>1</v>
+      </c>
+      <c r="F16" s="12">
         <v>1</v>
       </c>
       <c r="G16" s="6"/>
@@ -1146,12 +1150,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13">
-        <v>1</v>
-      </c>
-      <c r="F17" s="13"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12">
+        <v>1</v>
+      </c>
+      <c r="F17" s="12"/>
       <c r="G17" s="6"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1170,16 +1174,16 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C18" s="14">
-        <v>1</v>
-      </c>
-      <c r="D18" s="13">
-        <v>1</v>
-      </c>
-      <c r="E18" s="13">
-        <v>1</v>
-      </c>
-      <c r="F18" s="13">
+      <c r="C18" s="13">
+        <v>1</v>
+      </c>
+      <c r="D18" s="12">
+        <v>1</v>
+      </c>
+      <c r="E18" s="12">
+        <v>1</v>
+      </c>
+      <c r="F18" s="12">
         <v>1</v>
       </c>
       <c r="G18" s="6"/>
@@ -1192,16 +1196,16 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C19" s="14">
-        <v>1</v>
-      </c>
-      <c r="D19" s="13">
-        <v>1</v>
-      </c>
-      <c r="E19" s="13">
-        <v>1</v>
-      </c>
-      <c r="F19" s="13">
+      <c r="C19" s="13">
+        <v>1</v>
+      </c>
+      <c r="D19" s="12">
+        <v>1</v>
+      </c>
+      <c r="E19" s="12">
+        <v>1</v>
+      </c>
+      <c r="F19" s="12">
         <v>1</v>
       </c>
       <c r="G19" s="6"/>
@@ -1214,14 +1218,14 @@
         <f>IF(C20=1,1,0)+IF(D20=1,2,0)+IF(E20=1,4,0)+IF(F20=1,8,0)</f>
         <v>3</v>
       </c>
-      <c r="C20" s="15">
-        <v>1</v>
-      </c>
-      <c r="D20" s="14">
-        <v>1</v>
-      </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="C20" s="14">
+        <v>1</v>
+      </c>
+      <c r="D20" s="13">
+        <v>1</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
@@ -1232,14 +1236,14 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C21" s="15">
-        <v>1</v>
-      </c>
-      <c r="D21" s="14">
-        <v>1</v>
-      </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="C21" s="14">
+        <v>1</v>
+      </c>
+      <c r="D21" s="13">
+        <v>1</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
@@ -1250,14 +1254,14 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C22" s="15">
-        <v>1</v>
-      </c>
-      <c r="D22" s="14">
-        <v>1</v>
-      </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="C22" s="14">
+        <v>1</v>
+      </c>
+      <c r="D22" s="13">
+        <v>1</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
@@ -1268,17 +1272,35 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C23" s="15">
-        <v>1</v>
-      </c>
-      <c r="D23" s="14">
-        <v>1</v>
-      </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14">
+      <c r="C23" s="14">
+        <v>1</v>
+      </c>
+      <c r="D23" s="13">
+        <v>1</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13">
         <v>1</v>
       </c>
       <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C24" s="14">
+        <v>1</v>
+      </c>
+      <c r="D24" s="13">
+        <v>1</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1292,10 +1314,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1314,13 +1336,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="1">
@@ -1353,9 +1375,9 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1396,20 +1418,20 @@
         <f>L1-B3</f>
         <v>248</v>
       </c>
-      <c r="D3" s="16">
-        <v>1</v>
-      </c>
-      <c r="E3" s="16">
-        <v>1</v>
-      </c>
-      <c r="F3" s="16">
-        <v>1</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
+      <c r="D3" s="15">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15">
+        <v>1</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
       <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1424,20 +1446,20 @@
         <f>L1-B4</f>
         <v>248</v>
       </c>
-      <c r="D4" s="16">
-        <v>1</v>
-      </c>
-      <c r="E4" s="16">
-        <v>1</v>
-      </c>
-      <c r="F4" s="16">
-        <v>1</v>
-      </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
+      <c r="D4" s="15">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15">
+        <v>1</v>
+      </c>
+      <c r="F4" s="15">
+        <v>1</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1452,22 +1474,22 @@
         <f>L1-B5</f>
         <v>240</v>
       </c>
-      <c r="D5" s="16">
-        <v>1</v>
-      </c>
-      <c r="E5" s="16">
-        <v>1</v>
-      </c>
-      <c r="F5" s="16">
-        <v>1</v>
-      </c>
-      <c r="G5" s="16">
-        <v>1</v>
-      </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
+      <c r="D5" s="15">
+        <v>1</v>
+      </c>
+      <c r="E5" s="15">
+        <v>1</v>
+      </c>
+      <c r="F5" s="15">
+        <v>1</v>
+      </c>
+      <c r="G5" s="15">
+        <v>1</v>
+      </c>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1482,16 +1504,16 @@
         <f>L1-B6</f>
         <v>254</v>
       </c>
-      <c r="D6" s="16">
-        <v>1</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="D6" s="15">
+        <v>1</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1506,18 +1528,18 @@
         <f>L1-B7</f>
         <v>250</v>
       </c>
-      <c r="D7" s="16">
-        <v>1</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16">
-        <v>1</v>
-      </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+      <c r="D7" s="15">
+        <v>1</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15">
+        <v>1</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -1532,18 +1554,18 @@
         <f>L1-B8</f>
         <v>250</v>
       </c>
-      <c r="D8" s="16">
-        <v>1</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16">
-        <v>1</v>
-      </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
+      <c r="D8" s="15">
+        <v>1</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15">
+        <v>1</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1558,20 +1580,20 @@
         <f>L1-B9</f>
         <v>248</v>
       </c>
-      <c r="D9" s="16">
-        <v>1</v>
-      </c>
-      <c r="E9" s="16">
-        <v>1</v>
-      </c>
-      <c r="F9" s="16">
-        <v>1</v>
-      </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="D9" s="15">
+        <v>1</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1</v>
+      </c>
+      <c r="F9" s="15">
+        <v>1</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1586,16 +1608,16 @@
         <f>L1-B10</f>
         <v>254</v>
       </c>
-      <c r="D10" s="16">
-        <v>1</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
       <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1610,18 +1632,18 @@
         <f>L1-B11</f>
         <v>250</v>
       </c>
-      <c r="D11" s="16">
-        <v>1</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16">
-        <v>1</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="D11" s="15">
+        <v>1</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15">
+        <v>1</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1636,20 +1658,20 @@
         <f>L1-B12</f>
         <v>248</v>
       </c>
-      <c r="D12" s="16">
-        <v>1</v>
-      </c>
-      <c r="E12" s="16">
-        <v>1</v>
-      </c>
-      <c r="F12" s="16">
-        <v>1</v>
-      </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
+      <c r="D12" s="15">
+        <v>1</v>
+      </c>
+      <c r="E12" s="15">
+        <v>1</v>
+      </c>
+      <c r="F12" s="15">
+        <v>1</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1664,20 +1686,20 @@
         <f>L1-B13</f>
         <v>248</v>
       </c>
-      <c r="D13" s="16">
-        <v>1</v>
-      </c>
-      <c r="E13" s="16">
-        <v>1</v>
-      </c>
-      <c r="F13" s="16">
-        <v>1</v>
-      </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
+      <c r="D13" s="15">
+        <v>1</v>
+      </c>
+      <c r="E13" s="15">
+        <v>1</v>
+      </c>
+      <c r="F13" s="15">
+        <v>1</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1692,24 +1714,24 @@
         <f>L1-B14</f>
         <v>96</v>
       </c>
-      <c r="D14" s="16">
-        <v>1</v>
-      </c>
-      <c r="E14" s="16">
-        <v>1</v>
-      </c>
-      <c r="F14" s="16">
-        <v>1</v>
-      </c>
-      <c r="G14" s="16">
-        <v>1</v>
-      </c>
-      <c r="H14" s="16">
-        <v>1</v>
-      </c>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16">
+      <c r="D14" s="15">
+        <v>1</v>
+      </c>
+      <c r="E14" s="15">
+        <v>1</v>
+      </c>
+      <c r="F14" s="15">
+        <v>1</v>
+      </c>
+      <c r="G14" s="15">
+        <v>1</v>
+      </c>
+      <c r="H14" s="15">
+        <v>1</v>
+      </c>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15">
         <v>1</v>
       </c>
       <c r="L14" s="6"/>
@@ -1726,18 +1748,18 @@
         <f>L1-B15</f>
         <v>250</v>
       </c>
-      <c r="D15" s="16">
-        <v>1</v>
-      </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16">
-        <v>1</v>
-      </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="D15" s="15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -1752,26 +1774,26 @@
         <f>L1-B16</f>
         <v>64</v>
       </c>
-      <c r="D16" s="16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="16">
-        <v>1</v>
-      </c>
-      <c r="F16" s="16">
-        <v>1</v>
-      </c>
-      <c r="G16" s="16">
-        <v>1</v>
-      </c>
-      <c r="H16" s="16">
-        <v>1</v>
-      </c>
-      <c r="I16" s="16">
-        <v>1</v>
-      </c>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16">
+      <c r="D16" s="15">
+        <v>1</v>
+      </c>
+      <c r="E16" s="15">
+        <v>1</v>
+      </c>
+      <c r="F16" s="15">
+        <v>1</v>
+      </c>
+      <c r="G16" s="15">
+        <v>1</v>
+      </c>
+      <c r="H16" s="15">
+        <v>1</v>
+      </c>
+      <c r="I16" s="15">
+        <v>1</v>
+      </c>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15">
         <v>1</v>
       </c>
       <c r="L16" s="6"/>
@@ -1788,14 +1810,14 @@
         <f>L1-B17</f>
         <v>255</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -1810,20 +1832,20 @@
         <f>L1-B18</f>
         <v>248</v>
       </c>
-      <c r="D18" s="17">
-        <v>1</v>
-      </c>
-      <c r="E18" s="17">
-        <v>1</v>
-      </c>
-      <c r="F18" s="17">
-        <v>1</v>
-      </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
+      <c r="D18" s="16">
+        <v>1</v>
+      </c>
+      <c r="E18" s="16">
+        <v>1</v>
+      </c>
+      <c r="F18" s="16">
+        <v>1</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -1838,20 +1860,20 @@
         <f>L1-B19</f>
         <v>248</v>
       </c>
-      <c r="D19" s="17">
-        <v>1</v>
-      </c>
-      <c r="E19" s="17">
-        <v>1</v>
-      </c>
-      <c r="F19" s="17">
-        <v>1</v>
-      </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
+      <c r="D19" s="16">
+        <v>1</v>
+      </c>
+      <c r="E19" s="16">
+        <v>1</v>
+      </c>
+      <c r="F19" s="16">
+        <v>1</v>
+      </c>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -1866,16 +1888,16 @@
         <f>L1-B20</f>
         <v>254</v>
       </c>
-      <c r="D20" s="16">
-        <v>1</v>
-      </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
+      <c r="D20" s="15">
+        <v>1</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -1890,16 +1912,16 @@
         <f>L1-B21</f>
         <v>254</v>
       </c>
-      <c r="D21" s="16">
-        <v>1</v>
-      </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
+      <c r="D21" s="15">
+        <v>1</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
       <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -1914,16 +1936,16 @@
         <f>L1-B22</f>
         <v>254</v>
       </c>
-      <c r="D22" s="16">
-        <v>1</v>
-      </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
+      <c r="D22" s="15">
+        <v>1</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -1938,17 +1960,47 @@
         <f>L1-B23</f>
         <v>254</v>
       </c>
-      <c r="D23" s="16">
-        <v>1</v>
-      </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
+      <c r="D23" s="15">
+        <v>1</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
       <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="11">
+        <f>IF(Authority!C24=1,IF(D24=1,1,0)+IF(E24=1,2,0)+IF(F24=1,4,0)+IF(G24=1,8,0)+IF(H24=1,16,0)+IF(I24=1,32,0)+IF(J24=1,64,0)+IF(K24=1,128,0),0)</f>
+        <v>15</v>
+      </c>
+      <c r="C24" s="5">
+        <f>L1-B24</f>
+        <v>240</v>
+      </c>
+      <c r="D24" s="15">
+        <v>1</v>
+      </c>
+      <c r="E24" s="16">
+        <v>1</v>
+      </c>
+      <c r="F24" s="16">
+        <v>1</v>
+      </c>
+      <c r="G24" s="16">
+        <v>1</v>
+      </c>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1963,10 +2015,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1985,13 +2037,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="1">
@@ -2024,9 +2076,9 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
@@ -2067,20 +2119,20 @@
         <f>L1-B3</f>
         <v>248</v>
       </c>
-      <c r="D3" s="16">
-        <v>1</v>
-      </c>
-      <c r="E3" s="16">
-        <v>1</v>
-      </c>
-      <c r="F3" s="16">
-        <v>1</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
+      <c r="D3" s="15">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15">
+        <v>1</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
       <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -2095,20 +2147,20 @@
         <f>L1-B4</f>
         <v>248</v>
       </c>
-      <c r="D4" s="16">
-        <v>1</v>
-      </c>
-      <c r="E4" s="16">
-        <v>1</v>
-      </c>
-      <c r="F4" s="16">
-        <v>1</v>
-      </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
+      <c r="D4" s="15">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15">
+        <v>1</v>
+      </c>
+      <c r="F4" s="15">
+        <v>1</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -2123,16 +2175,16 @@
         <f>L1-B5</f>
         <v>255</v>
       </c>
-      <c r="D5" s="16">
-        <v>1</v>
-      </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
+      <c r="D5" s="15">
+        <v>1</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -2147,16 +2199,16 @@
         <f>L1-B6</f>
         <v>254</v>
       </c>
-      <c r="D6" s="16">
-        <v>1</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="D6" s="15">
+        <v>1</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -2171,18 +2223,18 @@
         <f>L1-B7</f>
         <v>250</v>
       </c>
-      <c r="D7" s="16">
-        <v>1</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16">
-        <v>1</v>
-      </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+      <c r="D7" s="15">
+        <v>1</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15">
+        <v>1</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -2197,18 +2249,18 @@
         <f>L1-B8</f>
         <v>255</v>
       </c>
-      <c r="D8" s="16">
-        <v>1</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16">
-        <v>1</v>
-      </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
+      <c r="D8" s="15">
+        <v>1</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15">
+        <v>1</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -2223,18 +2275,18 @@
         <f>L1-B9</f>
         <v>250</v>
       </c>
-      <c r="D9" s="16">
-        <v>1</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16">
-        <v>1</v>
-      </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="D9" s="15">
+        <v>1</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15">
+        <v>1</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -2249,16 +2301,16 @@
         <f>L1-B10</f>
         <v>254</v>
       </c>
-      <c r="D10" s="16">
-        <v>1</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
       <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -2273,18 +2325,18 @@
         <f>L1-B11</f>
         <v>250</v>
       </c>
-      <c r="D11" s="16">
-        <v>1</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16">
-        <v>1</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="D11" s="15">
+        <v>1</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15">
+        <v>1</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -2299,16 +2351,16 @@
         <f>L1-B12</f>
         <v>255</v>
       </c>
-      <c r="D12" s="16">
-        <v>1</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
+      <c r="D12" s="15">
+        <v>1</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -2323,16 +2375,16 @@
         <f>L1-B13</f>
         <v>255</v>
       </c>
-      <c r="D13" s="16">
-        <v>1</v>
-      </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
+      <c r="D13" s="15">
+        <v>1</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -2347,24 +2399,24 @@
         <f>L1-B14</f>
         <v>255</v>
       </c>
-      <c r="D14" s="16">
-        <v>1</v>
-      </c>
-      <c r="E14" s="16">
-        <v>1</v>
-      </c>
-      <c r="F14" s="16">
-        <v>1</v>
-      </c>
-      <c r="G14" s="16">
-        <v>1</v>
-      </c>
-      <c r="H14" s="16">
-        <v>1</v>
-      </c>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16">
+      <c r="D14" s="15">
+        <v>1</v>
+      </c>
+      <c r="E14" s="15">
+        <v>1</v>
+      </c>
+      <c r="F14" s="15">
+        <v>1</v>
+      </c>
+      <c r="G14" s="15">
+        <v>1</v>
+      </c>
+      <c r="H14" s="15">
+        <v>1</v>
+      </c>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15">
         <v>1</v>
       </c>
       <c r="L14" s="6"/>
@@ -2381,18 +2433,18 @@
         <f>L1-B15</f>
         <v>250</v>
       </c>
-      <c r="D15" s="16">
-        <v>1</v>
-      </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16">
-        <v>1</v>
-      </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="D15" s="15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -2407,16 +2459,16 @@
         <f>L1-B16</f>
         <v>254</v>
       </c>
-      <c r="D16" s="16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
+      <c r="D16" s="15">
+        <v>1</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -2431,14 +2483,14 @@
         <f>L1-B17</f>
         <v>255</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -2453,18 +2505,18 @@
         <f>L1-B18</f>
         <v>252</v>
       </c>
-      <c r="D18" s="17">
-        <v>1</v>
-      </c>
-      <c r="E18" s="17">
-        <v>1</v>
-      </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
+      <c r="D18" s="16">
+        <v>1</v>
+      </c>
+      <c r="E18" s="16">
+        <v>1</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -2479,18 +2531,18 @@
         <f>L1-B19</f>
         <v>252</v>
       </c>
-      <c r="D19" s="17">
-        <v>1</v>
-      </c>
-      <c r="E19" s="17">
-        <v>1</v>
-      </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
+      <c r="D19" s="16">
+        <v>1</v>
+      </c>
+      <c r="E19" s="16">
+        <v>1</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -2505,22 +2557,22 @@
         <f>L1-B20</f>
         <v>240</v>
       </c>
-      <c r="D20" s="16">
-        <v>1</v>
-      </c>
-      <c r="E20" s="17">
-        <v>1</v>
-      </c>
-      <c r="F20" s="17">
-        <v>1</v>
-      </c>
-      <c r="G20" s="17">
-        <v>1</v>
-      </c>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
+      <c r="D20" s="15">
+        <v>1</v>
+      </c>
+      <c r="E20" s="16">
+        <v>1</v>
+      </c>
+      <c r="F20" s="16">
+        <v>1</v>
+      </c>
+      <c r="G20" s="16">
+        <v>1</v>
+      </c>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -2535,22 +2587,22 @@
         <f>L1-B21</f>
         <v>240</v>
       </c>
-      <c r="D21" s="16">
-        <v>1</v>
-      </c>
-      <c r="E21" s="17">
-        <v>1</v>
-      </c>
-      <c r="F21" s="17">
-        <v>1</v>
-      </c>
-      <c r="G21" s="17">
-        <v>1</v>
-      </c>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
+      <c r="D21" s="15">
+        <v>1</v>
+      </c>
+      <c r="E21" s="16">
+        <v>1</v>
+      </c>
+      <c r="F21" s="16">
+        <v>1</v>
+      </c>
+      <c r="G21" s="16">
+        <v>1</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
       <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -2565,22 +2617,22 @@
         <f>L1-B22</f>
         <v>240</v>
       </c>
-      <c r="D22" s="16">
-        <v>1</v>
-      </c>
-      <c r="E22" s="17">
-        <v>1</v>
-      </c>
-      <c r="F22" s="17">
-        <v>1</v>
-      </c>
-      <c r="G22" s="17">
-        <v>1</v>
-      </c>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
+      <c r="D22" s="15">
+        <v>1</v>
+      </c>
+      <c r="E22" s="16">
+        <v>1</v>
+      </c>
+      <c r="F22" s="16">
+        <v>1</v>
+      </c>
+      <c r="G22" s="16">
+        <v>1</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -2595,23 +2647,53 @@
         <f>L1-B23</f>
         <v>240</v>
       </c>
-      <c r="D23" s="16">
-        <v>1</v>
-      </c>
-      <c r="E23" s="17">
-        <v>1</v>
-      </c>
-      <c r="F23" s="17">
-        <v>1</v>
-      </c>
-      <c r="G23" s="17">
-        <v>1</v>
-      </c>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
+      <c r="D23" s="15">
+        <v>1</v>
+      </c>
+      <c r="E23" s="16">
+        <v>1</v>
+      </c>
+      <c r="F23" s="16">
+        <v>1</v>
+      </c>
+      <c r="G23" s="16">
+        <v>1</v>
+      </c>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
       <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="11">
+        <f>IF(Authority!D24=1,IF(D24=1,1,0)+IF(E24=1,2,0)+IF(F24=1,4,0)+IF(G24=1,8,0)+IF(H24=1,16,0)+IF(I24=1,32,0)+IF(J24=1,64,0)+IF(K24=1,128,0),0)</f>
+        <v>15</v>
+      </c>
+      <c r="C24" s="5">
+        <f>L1-B24</f>
+        <v>240</v>
+      </c>
+      <c r="D24" s="15">
+        <v>1</v>
+      </c>
+      <c r="E24" s="16">
+        <v>1</v>
+      </c>
+      <c r="F24" s="16">
+        <v>1</v>
+      </c>
+      <c r="G24" s="16">
+        <v>1</v>
+      </c>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2626,10 +2708,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2648,13 +2730,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="1">
@@ -2687,9 +2769,9 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
@@ -2730,20 +2812,20 @@
         <f>L1-B3</f>
         <v>248</v>
       </c>
-      <c r="D3" s="16">
-        <v>1</v>
-      </c>
-      <c r="E3" s="16">
-        <v>1</v>
-      </c>
-      <c r="F3" s="16">
-        <v>1</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
+      <c r="D3" s="15">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15">
+        <v>1</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
       <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -2758,20 +2840,20 @@
         <f>L1-B4</f>
         <v>255</v>
       </c>
-      <c r="D4" s="16">
-        <v>1</v>
-      </c>
-      <c r="E4" s="16">
-        <v>1</v>
-      </c>
-      <c r="F4" s="16">
-        <v>1</v>
-      </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
+      <c r="D4" s="15">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15">
+        <v>1</v>
+      </c>
+      <c r="F4" s="15">
+        <v>1</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -2786,16 +2868,16 @@
         <f>L1-B5</f>
         <v>255</v>
       </c>
-      <c r="D5" s="16">
-        <v>1</v>
-      </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
+      <c r="D5" s="15">
+        <v>1</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -2810,16 +2892,16 @@
         <f>L1-B6</f>
         <v>254</v>
       </c>
-      <c r="D6" s="16">
-        <v>1</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="D6" s="15">
+        <v>1</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -2834,18 +2916,18 @@
         <f>L1-B7</f>
         <v>255</v>
       </c>
-      <c r="D7" s="16">
-        <v>1</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16">
-        <v>1</v>
-      </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+      <c r="D7" s="15">
+        <v>1</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15">
+        <v>1</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -2860,18 +2942,18 @@
         <f>L1-B8</f>
         <v>255</v>
       </c>
-      <c r="D8" s="16">
-        <v>1</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16">
-        <v>1</v>
-      </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
+      <c r="D8" s="15">
+        <v>1</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15">
+        <v>1</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -2886,18 +2968,18 @@
         <f>L1-B9</f>
         <v>250</v>
       </c>
-      <c r="D9" s="16">
-        <v>1</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16">
-        <v>1</v>
-      </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="D9" s="15">
+        <v>1</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15">
+        <v>1</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -2912,16 +2994,16 @@
         <f>L1-B10</f>
         <v>254</v>
       </c>
-      <c r="D10" s="16">
-        <v>1</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
       <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -2936,18 +3018,18 @@
         <f>L1-B11</f>
         <v>250</v>
       </c>
-      <c r="D11" s="16">
-        <v>1</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16">
-        <v>1</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="D11" s="15">
+        <v>1</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15">
+        <v>1</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -2962,16 +3044,16 @@
         <f>L1-B12</f>
         <v>255</v>
       </c>
-      <c r="D12" s="16">
-        <v>1</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
+      <c r="D12" s="15">
+        <v>1</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -2986,16 +3068,16 @@
         <f>L1-B13</f>
         <v>255</v>
       </c>
-      <c r="D13" s="16">
-        <v>1</v>
-      </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
+      <c r="D13" s="15">
+        <v>1</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -3010,24 +3092,24 @@
         <f>L1-B14</f>
         <v>255</v>
       </c>
-      <c r="D14" s="16">
-        <v>1</v>
-      </c>
-      <c r="E14" s="16">
-        <v>1</v>
-      </c>
-      <c r="F14" s="16">
-        <v>1</v>
-      </c>
-      <c r="G14" s="16">
-        <v>1</v>
-      </c>
-      <c r="H14" s="16">
-        <v>1</v>
-      </c>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16">
+      <c r="D14" s="15">
+        <v>1</v>
+      </c>
+      <c r="E14" s="15">
+        <v>1</v>
+      </c>
+      <c r="F14" s="15">
+        <v>1</v>
+      </c>
+      <c r="G14" s="15">
+        <v>1</v>
+      </c>
+      <c r="H14" s="15">
+        <v>1</v>
+      </c>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15">
         <v>1</v>
       </c>
       <c r="L14" s="6"/>
@@ -3044,18 +3126,18 @@
         <f>L1-B15</f>
         <v>250</v>
       </c>
-      <c r="D15" s="16">
-        <v>1</v>
-      </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16">
-        <v>1</v>
-      </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="D15" s="15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -3070,16 +3152,16 @@
         <f>L1-B16</f>
         <v>254</v>
       </c>
-      <c r="D16" s="16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
+      <c r="D16" s="15">
+        <v>1</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -3094,18 +3176,18 @@
         <f>L1-B17</f>
         <v>252</v>
       </c>
-      <c r="D17" s="16">
-        <v>1</v>
-      </c>
-      <c r="E17" s="16">
-        <v>1</v>
-      </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
+      <c r="D17" s="15">
+        <v>1</v>
+      </c>
+      <c r="E17" s="15">
+        <v>1</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -3120,18 +3202,18 @@
         <f>L1-B18</f>
         <v>252</v>
       </c>
-      <c r="D18" s="17">
-        <v>1</v>
-      </c>
-      <c r="E18" s="17">
-        <v>1</v>
-      </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
+      <c r="D18" s="16">
+        <v>1</v>
+      </c>
+      <c r="E18" s="16">
+        <v>1</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -3146,18 +3228,18 @@
         <f>L1-B19</f>
         <v>252</v>
       </c>
-      <c r="D19" s="17">
-        <v>1</v>
-      </c>
-      <c r="E19" s="17">
-        <v>1</v>
-      </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
+      <c r="D19" s="16">
+        <v>1</v>
+      </c>
+      <c r="E19" s="16">
+        <v>1</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -3172,14 +3254,14 @@
         <f>L1-B20</f>
         <v>255</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -3194,14 +3276,14 @@
         <f>L1-B21</f>
         <v>255</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
       <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -3216,14 +3298,14 @@
         <f>L1-B22</f>
         <v>255</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -3238,15 +3320,37 @@
         <f>L1-B23</f>
         <v>255</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
       <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="11">
+        <f>IF(Authority!E24=1,IF(D24=1,1,0)+IF(E24=1,2,0)+IF(F24=1,4,0)+IF(G24=1,8,0)+IF(H24=1,16,0)+IF(I24=1,32,0)+IF(J24=1,64,0)+IF(K24=1,128,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="5">
+        <f>L1-B24</f>
+        <v>255</v>
+      </c>
+      <c r="D24" s="15"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3261,10 +3365,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B035F1-1F9F-45E4-B506-6754E54E97D7}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3283,13 +3387,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="1">
@@ -3322,9 +3426,9 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
@@ -3365,20 +3469,20 @@
         <f>L1-B3</f>
         <v>248</v>
       </c>
-      <c r="D3" s="16">
-        <v>1</v>
-      </c>
-      <c r="E3" s="16">
-        <v>1</v>
-      </c>
-      <c r="F3" s="16">
-        <v>1</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
+      <c r="D3" s="15">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15">
+        <v>1</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
       <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -3393,20 +3497,20 @@
         <f>L1-B4</f>
         <v>255</v>
       </c>
-      <c r="D4" s="16">
-        <v>1</v>
-      </c>
-      <c r="E4" s="16">
-        <v>1</v>
-      </c>
-      <c r="F4" s="16">
-        <v>1</v>
-      </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
+      <c r="D4" s="15">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15">
+        <v>1</v>
+      </c>
+      <c r="F4" s="15">
+        <v>1</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -3421,14 +3525,14 @@
         <f>L1-B5</f>
         <v>255</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -3443,14 +3547,14 @@
         <f>L1-B6</f>
         <v>255</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -3465,18 +3569,18 @@
         <f>L1-B7</f>
         <v>255</v>
       </c>
-      <c r="D7" s="16">
-        <v>1</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16">
-        <v>1</v>
-      </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+      <c r="D7" s="15">
+        <v>1</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15">
+        <v>1</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -3491,14 +3595,14 @@
         <f>L1-B8</f>
         <v>255</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -3513,18 +3617,18 @@
         <f>L1-B9</f>
         <v>250</v>
       </c>
-      <c r="D9" s="16">
-        <v>1</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16">
-        <v>1</v>
-      </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="D9" s="15">
+        <v>1</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15">
+        <v>1</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -3539,16 +3643,16 @@
         <f>L1-B10</f>
         <v>254</v>
       </c>
-      <c r="D10" s="16">
-        <v>1</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
       <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -3563,18 +3667,18 @@
         <f>L1-B11</f>
         <v>250</v>
       </c>
-      <c r="D11" s="16">
-        <v>1</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16">
-        <v>1</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="D11" s="15">
+        <v>1</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15">
+        <v>1</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -3589,14 +3693,14 @@
         <f>L1-B12</f>
         <v>255</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -3611,14 +3715,14 @@
         <f>L1-B13</f>
         <v>255</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -3633,14 +3737,14 @@
         <f>L1-B14</f>
         <v>255</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -3655,18 +3759,18 @@
         <f>L1-B15</f>
         <v>250</v>
       </c>
-      <c r="D15" s="16">
-        <v>1</v>
-      </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16">
-        <v>1</v>
-      </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="D15" s="15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -3681,16 +3785,16 @@
         <f>L1-B16</f>
         <v>254</v>
       </c>
-      <c r="D16" s="16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
+      <c r="D16" s="15">
+        <v>1</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -3705,14 +3809,14 @@
         <f>L1-B17</f>
         <v>255</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -3727,18 +3831,18 @@
         <f>L1-B18</f>
         <v>252</v>
       </c>
-      <c r="D18" s="17">
-        <v>1</v>
-      </c>
-      <c r="E18" s="17">
-        <v>1</v>
-      </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
+      <c r="D18" s="16">
+        <v>1</v>
+      </c>
+      <c r="E18" s="16">
+        <v>1</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -3753,18 +3857,18 @@
         <f>L1-B19</f>
         <v>252</v>
       </c>
-      <c r="D19" s="17">
-        <v>1</v>
-      </c>
-      <c r="E19" s="17">
-        <v>1</v>
-      </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
+      <c r="D19" s="16">
+        <v>1</v>
+      </c>
+      <c r="E19" s="16">
+        <v>1</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -3779,14 +3883,14 @@
         <f>L1-B20</f>
         <v>255</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -3801,14 +3905,14 @@
         <f>L1-B21</f>
         <v>255</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
       <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -3823,14 +3927,14 @@
         <f>L1-B22</f>
         <v>255</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -3845,19 +3949,45 @@
         <f>L1-B23</f>
         <v>252</v>
       </c>
-      <c r="D23" s="16">
-        <v>1</v>
-      </c>
-      <c r="E23" s="17">
-        <v>1</v>
-      </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
+      <c r="D23" s="15">
+        <v>1</v>
+      </c>
+      <c r="E23" s="16">
+        <v>1</v>
+      </c>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
       <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="11">
+        <f>IF(Authority!F24=1,IF(D24=1,1,0)+IF(E24=1,2,0)+IF(F24=1,4,0)+IF(G24=1,8,0)+IF(H24=1,16,0)+IF(I24=1,32,0)+IF(J24=1,64,0)+IF(K24=1,128,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="5">
+        <f>L1-B24</f>
+        <v>255</v>
+      </c>
+      <c r="D24" s="15">
+        <v>1</v>
+      </c>
+      <c r="E24" s="16">
+        <v>1</v>
+      </c>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
- fixing bug migration for mongodb - add new lookup for brand data and logo
</commit_message>
<xml_diff>
--- a/SecurityMatrix.xlsx
+++ b/SecurityMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\GAI\vidmov-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3230F71-64DA-4DDE-9AF7-56A2C01A6063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F284FA-DEEB-4B78-979E-3E3814E5DF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Authority" sheetId="1" r:id="rId1"/>
@@ -283,10 +283,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,10 +702,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1">
@@ -734,8 +734,8 @@
       <c r="Q1"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1298,8 +1298,8 @@
       <c r="D24" s="13">
         <v>1</v>
       </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
       <c r="G24" s="6"/>
     </row>
   </sheetData>
@@ -1316,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1336,13 +1336,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="1">
@@ -1375,9 +1375,9 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1652,11 +1652,11 @@
       </c>
       <c r="B12" s="5">
         <f>IF(Authority!C12=1,IF(D12=1,1,0)+IF(E12=1,2,0)+IF(F12=1,4,0)+IF(G12=1,8,0)+IF(H12=1,16,0)+IF(I12=1,32,0)+IF(J12=1,64,0)+IF(K12=1,128,0),0)</f>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C12" s="5">
         <f>L1-B12</f>
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D12" s="15">
         <v>1</v>
@@ -1667,7 +1667,9 @@
       <c r="F12" s="15">
         <v>1</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="15">
+        <v>1</v>
+      </c>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
@@ -1680,11 +1682,11 @@
       </c>
       <c r="B13" s="5">
         <f>IF(Authority!C13=1,IF(D13=1,1,0)+IF(E13=1,2,0)+IF(F13=1,4,0)+IF(G13=1,8,0)+IF(H13=1,16,0)+IF(I13=1,32,0)+IF(J13=1,64,0)+IF(K13=1,128,0),0)</f>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C13" s="5">
         <f>L1-B13</f>
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D13" s="15">
         <v>1</v>
@@ -1695,7 +1697,9 @@
       <c r="F13" s="15">
         <v>1</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="15">
+        <v>1</v>
+      </c>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
@@ -2037,13 +2041,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="1">
@@ -2076,9 +2080,9 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
@@ -2730,13 +2734,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="1">
@@ -2769,9 +2773,9 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
@@ -3367,7 +3371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B035F1-1F9F-45E4-B506-6754E54E97D7}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
@@ -3387,13 +3391,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="1">
@@ -3426,9 +3430,9 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="3" t="s">
         <v>17</v>
       </c>

</xml_diff>